<commit_message>
customer uploading / API initial plan
</commit_message>
<xml_diff>
--- a/public/templates/customer-upload-template.xlsx
+++ b/public/templates/customer-upload-template.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20399"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E58ED5-FA34-4836-916E-FDCF92238A71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D2516A-629F-402B-83A4-A183862E6788}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Customer List</t>
   </si>
@@ -44,13 +44,25 @@
   </si>
   <si>
     <t>SAM</t>
+  </si>
+  <si>
+    <t>CHANNEL CODE</t>
+  </si>
+  <si>
+    <t>CHANNEL NAME</t>
+  </si>
+  <si>
+    <t>DEPT</t>
+  </si>
+  <si>
+    <t>DEPARTMENT STORE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,8 +82,16 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -81,6 +101,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC0C0C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -97,7 +123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -106,6 +132,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -397,14 +427,16 @@
     <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -414,11 +446,17 @@
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="E2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>100001</v>
       </c>
@@ -430,10 +468,16 @@
       </c>
       <c r="D3" t="s">
         <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
customer new template uploading
</commit_message>
<xml_diff>
--- a/public/templates/customer-upload-template.xlsx
+++ b/public/templates/customer-upload-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20409"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D2516A-629F-402B-83A4-A183862E6788}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30728B5D-6229-4E0E-AE67-F5BF4DB041E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Customer List</t>
   </si>
@@ -56,6 +56,30 @@
   </si>
   <si>
     <t>DEPARTMENT STORE</t>
+  </si>
+  <si>
+    <t>PROVINCE</t>
+  </si>
+  <si>
+    <t>CITY/TOWN</t>
+  </si>
+  <si>
+    <t>BARANGAY</t>
+  </si>
+  <si>
+    <t>STREET</t>
+  </si>
+  <si>
+    <t>MANILA</t>
+  </si>
+  <si>
+    <t>MAKATI</t>
+  </si>
+  <si>
+    <t>SAN ANTONIO</t>
+  </si>
+  <si>
+    <t>ARANGA</t>
   </si>
 </sst>
 </file>
@@ -416,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,12 +455,12 @@
     <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -455,8 +479,20 @@
       <c r="F2" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>100001</v>
       </c>
@@ -474,6 +510,18 @@
       </c>
       <c r="F3" t="s">
         <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add postal code to customer module
</commit_message>
<xml_diff>
--- a/public/templates/customer-upload-template.xlsx
+++ b/public/templates/customer-upload-template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20409"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30728B5D-6229-4E0E-AE67-F5BF4DB041E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C464FF-64FE-496C-AFA4-6DAD1E82527B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Customer List</t>
   </si>
@@ -37,12 +37,6 @@
     <t>SALESMAN CODE</t>
   </si>
   <si>
-    <t>SAMPLE CUSTOMER</t>
-  </si>
-  <si>
-    <t>BRGY. 1234 SAMPLE CITY</t>
-  </si>
-  <si>
     <t>SAM</t>
   </si>
   <si>
@@ -70,16 +64,28 @@
     <t>STREET</t>
   </si>
   <si>
-    <t>MANILA</t>
-  </si>
-  <si>
-    <t>MAKATI</t>
-  </si>
-  <si>
     <t>SAN ANTONIO</t>
   </si>
   <si>
     <t>ARANGA</t>
+  </si>
+  <si>
+    <t>MAKATI CITY</t>
+  </si>
+  <si>
+    <t>METRO MANILA</t>
+  </si>
+  <si>
+    <t>00000001</t>
+  </si>
+  <si>
+    <t>HA - House Account</t>
+  </si>
+  <si>
+    <t>PASIG</t>
+  </si>
+  <si>
+    <t>POSTAL CODE</t>
   </si>
 </sst>
 </file>
@@ -147,19 +153,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,88 +457,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="5"/>
+    <col min="5" max="5" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="16.28515625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="5" t="s">
+      <c r="G3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>100001</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" t="s">
-        <v>19</v>
+      <c r="K3" s="5">
+        <v>1203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>